<commit_message>
Atualização da base de dados Tabela final.xlsx
</commit_message>
<xml_diff>
--- a/Tabela final.xlsx
+++ b/Tabela final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\IA_Industria\incompatibilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8765B9D-D030-418F-9420-50D42B8742DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB88CD45-691E-4DC9-9680-9650071CEA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Dados" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Amina!$B$1:$H$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base_Dados!$B$1:$E$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base_Dados!$A$1:$G$107</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3716,6 +3716,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G107" xr:uid="{44DA4105-2C02-408D-BE9E-32A30E90C270}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>